<commit_message>
Ajuste de layout para impressao.
</commit_message>
<xml_diff>
--- a/Massa de dados/Visualizacoes Assunto-DiaSemana-hora.xlsx
+++ b/Massa de dados/Visualizacoes Assunto-DiaSemana-hora.xlsx
@@ -1372,11 +1372,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42602880"/>
-        <c:axId val="42604416"/>
+        <c:axId val="97549696"/>
+        <c:axId val="97555584"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="42602880"/>
+        <c:axId val="97549696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1386,7 +1386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42604416"/>
+        <c:crossAx val="97555584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1394,7 +1394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42604416"/>
+        <c:axId val="97555584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,7 +1405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42602880"/>
+        <c:crossAx val="97549696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1422,7 +1422,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1431,16 +1431,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1751,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,7 +2413,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>